<commit_message>
Versión 5.0 con la incorporación de BEES. Cambios menores requeridos
</commit_message>
<xml_diff>
--- a/output/assets/credenciales.xlsx
+++ b/output/assets/credenciales.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
@@ -49,7 +49,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,15 +57,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,63 +426,112 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col width="38.140625" customWidth="1" min="1" max="1"/>
     <col width="52.140625" customWidth="1" min="2" max="2"/>
-    <col width="30.42578125" customWidth="1" min="3" max="3"/>
+    <col width="111.5703125" customWidth="1" min="3" max="3"/>
     <col width="109.7109375" customWidth="1" min="4" max="4"/>
+    <col width="113.7109375" customWidth="1" min="6" max="6"/>
+    <col width="31.42578125" customWidth="1" min="7" max="7"/>
+    <col width="101.5703125" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>CORREO ELECTRÓNICO MAXICONSUMO</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="inlineStr"/>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>CONTRASEÑA MAXICONSUMO</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr"/>
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>NOMBRE DE USUARIO</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>CONTRASEÑA ENCRIPTADA</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>CORREO ELECTRÓNICO LA SERENÍSIMA</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>*78TZOkrnGG2JSdiMI2raPg==*Ug18e/Yj2xcWHEhDu+VAMg==*0/2Es8zSW9KPar5D8p77vQ==</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>CONTRASEÑA LA SERENÍSIMA</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>*yUg9OwJkzd9n48NpKeSORQ==*lPI/ZatGF6OXHpWzzk0GMQ==*pcT6ZwLOhfpXhEQvkxy0cg==</t>
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>MAXICONSUMO</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>orlando.piccinini@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" s="3" t="inlineStr">
+        <is>
+          <t>26TBDyfahsU=*kVpqWxsj5NswRl9AYd9qVw==*Ok3UyLr0xbq0hjgxP0lomw==*NepodkMzbVYH+ModcC9Sgw==</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="1" t="n"/>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>LA SERENÍSIMA</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>orlando.piccinini@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>7bwYIZivWO4dVRM=*mWprFGvNLOSV5+crKLSdxQ==*lhWQVj7MPOLpUA4Q8ciZ3Q==*q7T1Qa4n1CiByRrvIilD0g==</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>BEES (GRAL. ALVEAR)</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>2625404916</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>ddALT7mE3UQwH+DgsjKs900=*XX5AKld2q0bF52DUbAnM8w==*75+mUm0SnqACoKlKdheVgQ==*SsCetcMJvyJU29lez1AvQA==</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>BEES (SAN RAFAEL)</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>1158108611</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>BXDa7+m0Z3fg*sOGWT/rynsrO5dtvUe7tgw==*qAs8nFu3/+r9znWBh8KsUA==*eescdr4iBwPxuRun34hgZg==</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="C6" s="1" t="n"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B2" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="C2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>

</xml_diff>